<commit_message>
Excel utility test 03 march
</commit_message>
<xml_diff>
--- a/testdata/Excel_testData.xlsx
+++ b/testdata/Excel_testData.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{43A7B25B-DCB8-46DE-A669-A643AF3D01EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Cucumber6Series\CucumberPOMDesign\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13592B04-4DBC-48DD-8C8B-150762B25097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="23280" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ContactUS" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -385,7 +389,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>